<commit_message>
updated Acer experimental temps
</commit_message>
<xml_diff>
--- a/ED50/Acer_Mote_Genets_ED50.xlsx
+++ b/ED50/Acer_Mote_Genets_ED50.xlsx
@@ -1,71 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2917054de0bc48a0/Documents/Barshis_Lab/2021-June_Mote/ED50/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_EE65FDCE8F79A8D366075C52F3C3A2B3324A9EBF" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6AC30A73-9137-45AD-ACE8-C7BD5B31942F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Genotype</t>
-  </si>
-  <si>
-    <t>RossED50</t>
-  </si>
-  <si>
-    <t>T3ED50</t>
-  </si>
-  <si>
-    <t>T4ED50</t>
-  </si>
-  <si>
-    <t>T5ED50</t>
-  </si>
-  <si>
-    <t>07</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>62</t>
-  </si>
-  <si>
-    <t>CM5</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,14 +63,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -167,7 +109,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -199,27 +141,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -251,24 +175,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -444,166 +350,190 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Genotype</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>RossED50</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>T3ED50</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>T4ED50</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>T5ED50</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>07</t>
+        </is>
       </c>
       <c r="B2">
         <v>35.94</v>
       </c>
       <c r="C2">
-        <v>37.175076011735769</v>
+        <v>35.1593311241428</v>
       </c>
       <c r="D2">
-        <v>37.466675098287347</v>
+        <v>35.4477469890687</v>
       </c>
       <c r="E2">
-        <v>38.331697453354181</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
+        <v>36.31451605236354</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
       </c>
       <c r="B3">
-        <v>35.700000000000003</v>
+        <v>35.7</v>
       </c>
       <c r="C3">
-        <v>36.366153989034501</v>
+        <v>34.59176383833191</v>
       </c>
       <c r="D3">
-        <v>37.145046669428091</v>
+        <v>35.16370569644732</v>
       </c>
       <c r="E3">
-        <v>37.510879697987733</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
+        <v>35.50413325302423</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
       </c>
       <c r="B4">
         <v>36.42</v>
       </c>
       <c r="C4">
-        <v>37.026026534952351</v>
+        <v>35.01854086595885</v>
       </c>
       <c r="D4">
-        <v>37.293163107586537</v>
+        <v>35.27640446224537</v>
       </c>
       <c r="E4">
-        <v>37.542634129100662</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
+        <v>35.55175398183864</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
       </c>
       <c r="B5">
         <v>35.92</v>
       </c>
       <c r="C5">
-        <v>37.377615045317853</v>
+        <v>35.43858278505087</v>
       </c>
       <c r="D5">
-        <v>37.957241082075697</v>
+        <v>35.94748480797716</v>
       </c>
       <c r="E5">
-        <v>37.858939036210593</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>9</v>
+        <v>35.83001118047966</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
       </c>
       <c r="B6">
         <v>35.32</v>
       </c>
       <c r="C6">
-        <v>37.050243934599507</v>
+        <v>35.04164892766131</v>
       </c>
       <c r="D6">
-        <v>37.521462261175337</v>
+        <v>35.50543771969571</v>
       </c>
       <c r="E6">
-        <v>37.935751347205127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
+        <v>35.78730468150815</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
       </c>
       <c r="B7">
-        <v>36.049999999999997</v>
+        <v>36.05</v>
       </c>
       <c r="C7">
-        <v>36.994215755404127</v>
+        <v>34.99394777464237</v>
       </c>
       <c r="D7">
-        <v>37.253591162099738</v>
+        <v>35.23905644259535</v>
       </c>
       <c r="E7">
-        <v>37.541076380969791</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>11</v>
+        <v>35.53420034404618</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="B8">
         <v>35.64</v>
       </c>
       <c r="C8">
-        <v>37.34503942067677</v>
+        <v>35.34051760175029</v>
       </c>
       <c r="D8">
-        <v>36.987715917430492</v>
+        <v>35.00539928930295</v>
       </c>
       <c r="E8">
-        <v>37.334539558409112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>12</v>
+        <v>35.35020255626566</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>CM5</t>
+        </is>
       </c>
       <c r="B9">
         <v>35.44</v>
       </c>
       <c r="C9">
-        <v>37.867869828963237</v>
+        <v>35.86397961687468</v>
       </c>
       <c r="D9">
-        <v>37.840221326300359</v>
+        <v>35.83417374815685</v>
       </c>
       <c r="E9">
-        <v>38.079706716497903</v>
+        <v>36.05273260836525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated T3 DRC data
</commit_message>
<xml_diff>
--- a/ED50/Acer_Mote_Genets_ED50.xlsx
+++ b/ED50/Acer_Mote_Genets_ED50.xlsx
@@ -397,10 +397,10 @@
         <v>35.1593311241428</v>
       </c>
       <c r="D2">
-        <v>35.4477469890687</v>
+        <v>35.23671050776777</v>
       </c>
       <c r="E2">
-        <v>36.31451605236354</v>
+        <v>36.15439588328721</v>
       </c>
     </row>
     <row r="3">
@@ -416,10 +416,10 @@
         <v>34.59176383833191</v>
       </c>
       <c r="D3">
-        <v>35.16370569644732</v>
+        <v>34.95350722098058</v>
       </c>
       <c r="E3">
-        <v>35.50413325302423</v>
+        <v>35.10024149369163</v>
       </c>
     </row>
     <row r="4">
@@ -435,10 +435,10 @@
         <v>35.01854086595885</v>
       </c>
       <c r="D4">
-        <v>35.27640446224537</v>
+        <v>34.93877611932735</v>
       </c>
       <c r="E4">
-        <v>35.55175398183864</v>
+        <v>34.90285597640286</v>
       </c>
     </row>
     <row r="5">
@@ -454,10 +454,10 @@
         <v>35.43858278505087</v>
       </c>
       <c r="D5">
-        <v>35.94748480797716</v>
+        <v>35.32282634241693</v>
       </c>
       <c r="E5">
-        <v>35.83001118047966</v>
+        <v>35.35382334326526</v>
       </c>
     </row>
     <row r="6">
@@ -473,10 +473,10 @@
         <v>35.04164892766131</v>
       </c>
       <c r="D6">
-        <v>35.50543771969571</v>
+        <v>34.95869030693223</v>
       </c>
       <c r="E6">
-        <v>35.78730468150815</v>
+        <v>35.11888985603599</v>
       </c>
     </row>
     <row r="7">
@@ -492,10 +492,10 @@
         <v>34.99394777464237</v>
       </c>
       <c r="D7">
-        <v>35.23905644259535</v>
+        <v>35.03854759314339</v>
       </c>
       <c r="E7">
-        <v>35.53420034404618</v>
+        <v>34.99056870452858</v>
       </c>
     </row>
     <row r="8">
@@ -511,10 +511,10 @@
         <v>35.34051760175029</v>
       </c>
       <c r="D8">
-        <v>35.00539928930295</v>
+        <v>34.59192476885546</v>
       </c>
       <c r="E8">
-        <v>35.35020255626566</v>
+        <v>34.5203374798529</v>
       </c>
     </row>
     <row r="9">
@@ -530,10 +530,10 @@
         <v>35.86397961687468</v>
       </c>
       <c r="D9">
-        <v>35.83417374815685</v>
+        <v>35.39743386168312</v>
       </c>
       <c r="E9">
-        <v>36.05273260836525</v>
+        <v>35.39667167644611</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
calculate all Past ED50s per timepoint
</commit_message>
<xml_diff>
--- a/ED50/Acer_Mote_Genets_ED50.xlsx
+++ b/ED50/Acer_Mote_Genets_ED50.xlsx
@@ -1,21 +1,97 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2917054de0bc48a0/Documents/Barshis_Lab/2021-June_Mote/ED50/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_4E7DFDCE8F79A8D366075C52F31AEAF4EE988E27" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7CF20E43-71E4-4361-8E9B-5CBF889D7B7A}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+  <si>
+    <t>Genotype</t>
+  </si>
+  <si>
+    <t>RossED50</t>
+  </si>
+  <si>
+    <t>T3ED50</t>
+  </si>
+  <si>
+    <t>T4ED50</t>
+  </si>
+  <si>
+    <t>T5ED50</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>CM5</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>diff</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>avg-Ross</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,6 +139,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -109,7 +193,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -141,9 +225,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,6 +277,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -350,178 +470,309 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Genotype</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>RossED50</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>T3ED50</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>T4ED50</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>T5ED50</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>07</t>
-        </is>
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
       </c>
       <c r="B2">
         <v>35.94</v>
       </c>
       <c r="C2">
-        <v>35.1593311241428</v>
+        <v>35.159331124142803</v>
       </c>
       <c r="D2">
-        <v>35.23671050776777</v>
+        <v>35.236710507767768</v>
       </c>
       <c r="E2">
-        <v>36.15439588328721</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
+        <v>36.154395883287208</v>
+      </c>
+      <c r="F2">
+        <f>MIN(C2:E2)</f>
+        <v>35.159331124142803</v>
+      </c>
+      <c r="G2">
+        <f>MAX(C2:E2)</f>
+        <v>36.154395883287208</v>
+      </c>
+      <c r="H2">
+        <f>G2-F2</f>
+        <v>0.99506475914440529</v>
+      </c>
+      <c r="I2">
+        <f>AVERAGE(C2:E2)</f>
+        <v>35.516812505065928</v>
+      </c>
+      <c r="J2">
+        <f>I2-B2</f>
+        <v>-0.42318749493406926</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>35.7</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="C3">
-        <v>34.59176383833191</v>
+        <v>34.591763838331907</v>
       </c>
       <c r="D3">
-        <v>34.95350722098058</v>
+        <v>34.953507220980583</v>
       </c>
       <c r="E3">
-        <v>35.10024149369163</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
+        <v>35.100241493691627</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F12" si="0">MIN(C3:E3)</f>
+        <v>34.591763838331907</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G12" si="1">MAX(C3:E3)</f>
+        <v>35.100241493691627</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H12" si="2">G3-F3</f>
+        <v>0.50847765535971945</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I12" si="3">AVERAGE(C3:E3)</f>
+        <v>34.881837517668039</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J12" si="4">I3-B3</f>
+        <v>-0.81816248233196376</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
       </c>
       <c r="B4">
         <v>36.42</v>
       </c>
       <c r="C4">
-        <v>35.01854086595885</v>
+        <v>35.018540865958848</v>
       </c>
       <c r="D4">
-        <v>34.93877611932735</v>
+        <v>34.938776119327351</v>
       </c>
       <c r="E4">
-        <v>34.90285597640286</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>41</t>
-        </is>
+        <v>34.902855976402861</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>34.902855976402861</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>35.018540865958848</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="2"/>
+        <v>0.1156848895559861</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="3"/>
+        <v>34.953390987229689</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="4"/>
+        <v>-1.4666090127703129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
       </c>
       <c r="B5">
         <v>35.92</v>
       </c>
       <c r="C5">
-        <v>35.43858278505087</v>
+        <v>35.438582785050869</v>
       </c>
       <c r="D5">
-        <v>35.32282634241693</v>
+        <v>35.322826342416931</v>
       </c>
       <c r="E5">
-        <v>35.35382334326526</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
+        <v>35.353823343265262</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>35.322826342416931</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>35.438582785050869</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>0.1157564426339377</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="3"/>
+        <v>35.371744156911021</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="4"/>
+        <v>-0.54825584308898101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
       </c>
       <c r="B6">
         <v>35.32</v>
       </c>
       <c r="C6">
-        <v>35.04164892766131</v>
+        <v>35.041648927661313</v>
       </c>
       <c r="D6">
-        <v>34.95869030693223</v>
+        <v>34.958690306932233</v>
       </c>
       <c r="E6">
-        <v>35.11888985603599</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
+        <v>35.118889856035992</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>34.958690306932233</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>35.118889856035992</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>0.16019954910375844</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>35.039743030209848</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="4"/>
+        <v>-0.2802569697901518</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>36.05</v>
+        <v>36.049999999999997</v>
       </c>
       <c r="C7">
-        <v>34.99394777464237</v>
+        <v>34.993947774642372</v>
       </c>
       <c r="D7">
-        <v>35.03854759314339</v>
+        <v>35.038547593143392</v>
       </c>
       <c r="E7">
-        <v>34.99056870452858</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
+        <v>34.990568704528577</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>34.990568704528577</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>35.038547593143392</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>4.7978888614814252E-2</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>35.007688024104787</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="4"/>
+        <v>-1.0423119758952097</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
       </c>
       <c r="B8">
         <v>35.64</v>
       </c>
       <c r="C8">
-        <v>35.34051760175029</v>
+        <v>35.340517601750292</v>
       </c>
       <c r="D8">
-        <v>34.59192476885546</v>
+        <v>34.591924768855463</v>
       </c>
       <c r="E8">
-        <v>34.5203374798529</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>CM5</t>
-        </is>
+        <v>34.520337479852898</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>34.520337479852898</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>35.340517601750292</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>0.82018012189739409</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>34.817593283486218</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="4"/>
+        <v>-0.8224067165137825</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
       </c>
       <c r="B9">
         <v>35.44</v>
@@ -530,10 +781,153 @@
         <v>35.86397961687468</v>
       </c>
       <c r="D9">
-        <v>35.39743386168312</v>
+        <v>35.397433861683119</v>
       </c>
       <c r="E9">
-        <v>35.39667167644611</v>
+        <v>35.396671676446111</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>35.396671676446111</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>35.86397961687468</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>0.46730794042856871</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>35.552695051667968</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="4"/>
+        <v>0.11269505166796989</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <f>MIN(B2:B9)</f>
+        <v>35.32</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:E10" si="5">MIN(C2:C9)</f>
+        <v>34.591763838331907</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="5"/>
+        <v>34.591924768855463</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="5"/>
+        <v>34.520337479852898</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>34.520337479852898</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>34.591924768855463</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>7.1587289002565058E-2</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>34.568008695680092</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="4"/>
+        <v>-0.75199130431990824</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <f>MAX(B2:B9)</f>
+        <v>36.42</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:E11" si="6">MAX(C2:C9)</f>
+        <v>35.86397961687468</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="6"/>
+        <v>35.397433861683119</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="6"/>
+        <v>36.154395883287208</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>35.397433861683119</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>36.154395883287208</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>0.75696202160408887</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>35.805269787281667</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="4"/>
+        <v>-0.61473021271833517</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <f>B11-B10</f>
+        <v>1.1000000000000014</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:E12" si="7">C11-C10</f>
+        <v>1.2722157785427726</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="7"/>
+        <v>0.80550909282765559</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="7"/>
+        <v>1.6340584034343095</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.80550909282765559</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>1.6340584034343095</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>0.82854931060665393</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>1.2372610916015792</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="4"/>
+        <v>0.13726109160157773</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Past T3 sample time ED50 calculations
</commit_message>
<xml_diff>
--- a/ED50/Acer_Mote_Genets_ED50.xlsx
+++ b/ED50/Acer_Mote_Genets_ED50.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2917054de0bc48a0/Documents/Barshis_Lab/2021-June_Mote/ED50/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_4E7DFDCE8F79A8D366075C52F31AEAF4EE988E27" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7CF20E43-71E4-4361-8E9B-5CBF889D7B7A}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_4E7DFDCE8F79A8D366075C52F31AEAF4EE988E27" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{05DB15DF-DC97-451B-BBFE-0642CACAB45A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10968" yWindow="0" windowWidth="9888" windowHeight="11808" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>